<commit_message>
chart updates for AMDT 18
it includes SUP 14-16, 16-16, 17-16
</commit_message>
<xml_diff>
--- a/03_AD/MROC/RNAV SID AND STAR TABLES.xlsx
+++ b/03_AD/MROC/RNAV SID AND STAR TABLES.xlsx
@@ -13,17 +13,18 @@
   </bookViews>
   <sheets>
     <sheet name="COCOS2" sheetId="4" r:id="rId1"/>
-    <sheet name="SID COCOS7" sheetId="1" r:id="rId2"/>
-    <sheet name="TARCO 1" sheetId="2" r:id="rId3"/>
-    <sheet name="TARCO 2" sheetId="3" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
+    <sheet name="RNP AR RWY25" sheetId="6" r:id="rId2"/>
+    <sheet name="SID COCOS7" sheetId="1" r:id="rId3"/>
+    <sheet name="TARCO 1" sheetId="2" r:id="rId4"/>
+    <sheet name="TARCO 2" sheetId="3" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="381">
   <si>
     <t>095747.3N</t>
   </si>
@@ -1488,13 +1489,186 @@
   </si>
   <si>
     <t>PARRI</t>
+  </si>
+  <si>
+    <t>Designator</t>
+  </si>
+  <si>
+    <t>Path Descriptor</t>
+  </si>
+  <si>
+    <t>Fix Identifier
+(Waypoint Name)</t>
+  </si>
+  <si>
+    <t>Flyover</t>
+  </si>
+  <si>
+    <t>Course
+°M (°T)</t>
+  </si>
+  <si>
+    <t>Turn Direction</t>
+  </si>
+  <si>
+    <t>Altitude
+(ft)</t>
+  </si>
+  <si>
+    <t>Distance 
+(Nm)</t>
+  </si>
+  <si>
+    <t>Speed
+Limit (Kt)</t>
+  </si>
+  <si>
+    <t>Magnetic
+Variation</t>
+  </si>
+  <si>
+    <t>Vertical Angle/ Threshold Crossing Height</t>
+  </si>
+  <si>
+    <t>Navigation
+Performance</t>
+  </si>
+  <si>
+    <t>radius (NM)</t>
+  </si>
+  <si>
+    <t>Arc Center Fix</t>
+  </si>
+  <si>
+    <t>D/d</t>
+  </si>
+  <si>
+    <t>M/d</t>
+  </si>
+  <si>
+    <t>DECLINATION</t>
+  </si>
+  <si>
+    <t>IF</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>0°20' W</t>
+  </si>
+  <si>
+    <t>TF</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>-3.5°</t>
+  </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>-3.5°/50'</t>
+  </si>
+  <si>
+    <t>RNP W RWY25 (AR)</t>
+  </si>
+  <si>
+    <t>OC301
+(IAF)</t>
+  </si>
+  <si>
+    <t>OC303
+094827.8N
+0841455.2W</t>
+  </si>
+  <si>
+    <t>OC308</t>
+  </si>
+  <si>
+    <t>OC307
+095823.1N
+0840813.3W</t>
+  </si>
+  <si>
+    <t>RNP AR</t>
+  </si>
+  <si>
+    <t>OC305
+(FAF)</t>
+  </si>
+  <si>
+    <t>OC304
+(IF)</t>
+  </si>
+  <si>
+    <t>OC309
+MAPt (RWY25)</t>
+  </si>
+  <si>
+    <t>OC310
+(MHF)</t>
+  </si>
+  <si>
+    <t>3517/
+3427</t>
+  </si>
+  <si>
+    <t>095949.60N</t>
+  </si>
+  <si>
+    <t>0841200.98W</t>
+  </si>
+  <si>
+    <t>095236.5N</t>
+  </si>
+  <si>
+    <t>0843117.0W</t>
+  </si>
+  <si>
+    <t>094913.6N</t>
+  </si>
+  <si>
+    <t>0841847.6W</t>
+  </si>
+  <si>
+    <t>095204.5N</t>
+  </si>
+  <si>
+    <t>0841626.7W</t>
+  </si>
+  <si>
+    <t>095555.0N</t>
+  </si>
+  <si>
+    <t>0840710.9W</t>
+  </si>
+  <si>
+    <t>100053.3N</t>
+  </si>
+  <si>
+    <t>0840910.4W</t>
+  </si>
+  <si>
+    <t>018 (018)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1519,16 +1693,72 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -1791,11 +2021,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1865,6 +2115,62 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1959,6 +2265,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1994,6 +2317,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2531,9 +2871,597 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:P8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="5" width="15" customWidth="1"/>
+    <col min="16" max="17" width="13.140625" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" customWidth="1"/>
+    <col min="19" max="20" width="11.42578125" customWidth="1"/>
+    <col min="21" max="21" width="20.7109375" customWidth="1"/>
+    <col min="22" max="22" width="11.42578125" customWidth="1"/>
+    <col min="23" max="23" width="15.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>330</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>331</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>332</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>333</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>334</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>335</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>336</v>
+      </c>
+      <c r="J1" s="24" t="s">
+        <v>337</v>
+      </c>
+      <c r="K1" s="24" t="s">
+        <v>338</v>
+      </c>
+      <c r="L1" s="24" t="s">
+        <v>339</v>
+      </c>
+      <c r="M1" s="24" t="s">
+        <v>340</v>
+      </c>
+      <c r="N1" s="24" t="s">
+        <v>341</v>
+      </c>
+      <c r="O1" s="25" t="s">
+        <v>342</v>
+      </c>
+      <c r="P1" s="25" t="s">
+        <v>343</v>
+      </c>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="S1" s="26" t="s">
+        <v>344</v>
+      </c>
+      <c r="T1" s="26" t="s">
+        <v>345</v>
+      </c>
+      <c r="U1" s="27" t="s">
+        <v>346</v>
+      </c>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+    </row>
+    <row r="2" spans="1:23" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>357</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>347</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>358</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>355</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>348</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="I2" s="30">
+        <v>9000</v>
+      </c>
+      <c r="J2" s="38">
+        <v>3.2</v>
+      </c>
+      <c r="K2" s="29">
+        <v>230</v>
+      </c>
+      <c r="L2" s="31" t="s">
+        <v>349</v>
+      </c>
+      <c r="M2" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="N2" s="29" t="s">
+        <v>362</v>
+      </c>
+      <c r="O2" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="P2" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="32" t="s">
+        <v>348</v>
+      </c>
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
+      <c r="U2" s="28"/>
+      <c r="V2" s="28"/>
+      <c r="W2" s="28"/>
+    </row>
+    <row r="3" spans="1:23" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>357</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>350</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>322</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>372</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>373</v>
+      </c>
+      <c r="F3" s="29" t="s">
+        <v>355</v>
+      </c>
+      <c r="G3" s="42" t="s">
+        <v>380</v>
+      </c>
+      <c r="H3" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="I3" s="30">
+        <v>8568</v>
+      </c>
+      <c r="J3" s="36">
+        <v>3.2</v>
+      </c>
+      <c r="K3" s="29">
+        <v>210</v>
+      </c>
+      <c r="L3" s="31" t="s">
+        <v>349</v>
+      </c>
+      <c r="M3" s="30" t="s">
+        <v>352</v>
+      </c>
+      <c r="N3" s="29" t="s">
+        <v>362</v>
+      </c>
+      <c r="O3" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="P3" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="Q3" s="41"/>
+      <c r="R3" s="33" t="s">
+        <v>348</v>
+      </c>
+      <c r="S3" s="34">
+        <v>1</v>
+      </c>
+      <c r="T3" s="34">
+        <v>0</v>
+      </c>
+      <c r="U3" s="34">
+        <f>(S3+T3/60)</f>
+        <v>1</v>
+      </c>
+      <c r="V3" s="34" t="e">
+        <f>R3-U3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W3" s="34" t="e">
+        <f>TEXT(V3,"000")&amp;TEXT(R3," (000)")</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>357</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>353</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>364</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>374</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>375</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>355</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>348</v>
+      </c>
+      <c r="H4" s="29" t="s">
+        <v>354</v>
+      </c>
+      <c r="I4" s="30">
+        <v>8049</v>
+      </c>
+      <c r="J4" s="39">
+        <v>3.8</v>
+      </c>
+      <c r="K4" s="29">
+        <v>210</v>
+      </c>
+      <c r="L4" s="31" t="s">
+        <v>349</v>
+      </c>
+      <c r="M4" s="30" t="s">
+        <v>352</v>
+      </c>
+      <c r="N4" s="29" t="s">
+        <v>362</v>
+      </c>
+      <c r="O4" s="36">
+        <v>3.9</v>
+      </c>
+      <c r="P4" s="29" t="s">
+        <v>359</v>
+      </c>
+      <c r="Q4" s="41"/>
+      <c r="R4" s="33" t="s">
+        <v>348</v>
+      </c>
+      <c r="S4" s="34">
+        <v>1</v>
+      </c>
+      <c r="T4" s="34">
+        <v>0</v>
+      </c>
+      <c r="U4" s="34">
+        <f t="shared" ref="U4:U8" si="0">(S4+T4/60)</f>
+        <v>1</v>
+      </c>
+      <c r="V4" s="34" t="e">
+        <f t="shared" ref="V4:V8" si="1">R4-U4</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W4" s="34" t="e">
+        <f t="shared" ref="W4:W8" si="2">TEXT(V4,"000")&amp;TEXT(R4," (000)")</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
+        <v>357</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>350</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>363</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>376</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>377</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>355</v>
+      </c>
+      <c r="G5" s="31" t="str">
+        <f>W5</f>
+        <v>066 (067)</v>
+      </c>
+      <c r="H5" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="I5" s="30">
+        <v>7280</v>
+      </c>
+      <c r="J5" s="39">
+        <v>9.9</v>
+      </c>
+      <c r="K5" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="L5" s="31" t="s">
+        <v>349</v>
+      </c>
+      <c r="M5" s="30" t="s">
+        <v>352</v>
+      </c>
+      <c r="N5" s="29" t="s">
+        <v>362</v>
+      </c>
+      <c r="O5" s="35" t="s">
+        <v>348</v>
+      </c>
+      <c r="P5" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="Q5" s="41"/>
+      <c r="R5" s="33">
+        <v>67.289590000000004</v>
+      </c>
+      <c r="S5" s="34">
+        <v>1</v>
+      </c>
+      <c r="T5" s="34">
+        <v>0</v>
+      </c>
+      <c r="U5" s="34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="V5" s="34">
+        <f t="shared" si="1"/>
+        <v>66.289590000000004</v>
+      </c>
+      <c r="W5" s="34" t="str">
+        <f t="shared" si="2"/>
+        <v>066 (067)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
+        <v>357</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>353</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>360</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>378</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>379</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>355</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>348</v>
+      </c>
+      <c r="H6" s="29" t="s">
+        <v>351</v>
+      </c>
+      <c r="I6" s="30">
+        <v>4193</v>
+      </c>
+      <c r="J6" s="39">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="K6" s="29">
+        <v>165</v>
+      </c>
+      <c r="L6" s="31" t="s">
+        <v>349</v>
+      </c>
+      <c r="M6" s="30" t="s">
+        <v>352</v>
+      </c>
+      <c r="N6" s="29" t="s">
+        <v>362</v>
+      </c>
+      <c r="O6" s="29">
+        <v>2.7</v>
+      </c>
+      <c r="P6" s="29" t="s">
+        <v>361</v>
+      </c>
+      <c r="Q6" s="41"/>
+      <c r="R6" s="33" t="s">
+        <v>348</v>
+      </c>
+      <c r="S6" s="34">
+        <v>1</v>
+      </c>
+      <c r="T6" s="34">
+        <v>0</v>
+      </c>
+      <c r="U6" s="34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="V6" s="34" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W6" s="34" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
+        <v>357</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>350</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>365</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>368</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>369</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>355</v>
+      </c>
+      <c r="G7" s="31" t="str">
+        <f>W7</f>
+        <v>248 (249)</v>
+      </c>
+      <c r="H7" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="I7" s="37" t="s">
+        <v>367</v>
+      </c>
+      <c r="J7" s="39">
+        <v>3</v>
+      </c>
+      <c r="K7" s="43">
+        <v>248</v>
+      </c>
+      <c r="L7" s="31" t="s">
+        <v>349</v>
+      </c>
+      <c r="M7" s="30" t="s">
+        <v>356</v>
+      </c>
+      <c r="N7" s="29" t="s">
+        <v>362</v>
+      </c>
+      <c r="O7" s="35" t="s">
+        <v>348</v>
+      </c>
+      <c r="P7" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="Q7" s="41"/>
+      <c r="R7" s="33">
+        <v>249.36086</v>
+      </c>
+      <c r="S7" s="34">
+        <v>1</v>
+      </c>
+      <c r="T7" s="34">
+        <v>0</v>
+      </c>
+      <c r="U7" s="34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="V7" s="34">
+        <f t="shared" si="1"/>
+        <v>248.36086</v>
+      </c>
+      <c r="W7" s="34" t="str">
+        <f t="shared" si="2"/>
+        <v>248 (249)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>357</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>350</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>366</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>370</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>371</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>355</v>
+      </c>
+      <c r="G8" s="31" t="str">
+        <f>W8</f>
+        <v>248 (249)</v>
+      </c>
+      <c r="H8" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="I8" s="30">
+        <v>6500</v>
+      </c>
+      <c r="J8" s="39">
+        <v>20.3</v>
+      </c>
+      <c r="K8" s="29">
+        <v>230</v>
+      </c>
+      <c r="L8" s="31" t="s">
+        <v>349</v>
+      </c>
+      <c r="M8" s="30" t="s">
+        <v>352</v>
+      </c>
+      <c r="N8" s="29" t="s">
+        <v>362</v>
+      </c>
+      <c r="O8" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="P8" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="Q8" s="41"/>
+      <c r="R8" s="33">
+        <v>249.32705000000001</v>
+      </c>
+      <c r="S8" s="34">
+        <v>1</v>
+      </c>
+      <c r="T8" s="34">
+        <v>0</v>
+      </c>
+      <c r="U8" s="34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="V8" s="34">
+        <f t="shared" si="1"/>
+        <v>248.32705000000001</v>
+      </c>
+      <c r="W8" s="34" t="str">
+        <f t="shared" si="2"/>
+        <v>248 (249)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R14" s="33">
+        <v>11.225300000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
@@ -3022,7 +3950,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
@@ -3328,7 +4256,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
@@ -3644,7 +4572,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B6:C16"/>
   <sheetViews>

</xml_diff>